<commit_message>
v7 has additional axial reflector elements
</commit_message>
<xml_diff>
--- a/mcnp/lattice_comparison.xlsx
+++ b/mcnp/lattice_comparison.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="3 types" sheetId="1" r:id="rId1"/>
+    <sheet name="Plates" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="31">
   <si>
     <t>pitch (cm)</t>
   </si>
@@ -69,12 +70,63 @@
   </si>
   <si>
     <t>Using PWR fuel dimensions as approximate guesses</t>
+  </si>
+  <si>
+    <t>clad width</t>
+  </si>
+  <si>
+    <t>plate per assm.</t>
+  </si>
+  <si>
+    <t>fuel</t>
+  </si>
+  <si>
+    <t>clad</t>
+  </si>
+  <si>
+    <t>coolant</t>
+  </si>
+  <si>
+    <t>Dims (cm)</t>
+  </si>
+  <si>
+    <t>height</t>
+  </si>
+  <si>
+    <t>clad width (cm)</t>
+  </si>
+  <si>
+    <t>v2</t>
+  </si>
+  <si>
+    <t>v5</t>
+  </si>
+  <si>
+    <t>assm. Fuel vol (cm^3)</t>
+  </si>
+  <si>
+    <t>assm. height</t>
+  </si>
+  <si>
+    <t>assm #</t>
+  </si>
+  <si>
+    <t>total fuel vol</t>
+  </si>
+  <si>
+    <t>channel thickness (cm)</t>
+  </si>
+  <si>
+    <t>v6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -112,9 +164,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -395,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:I12"/>
+  <dimension ref="B1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -612,8 +668,479 @@
         <v>2.4057117020236598</v>
       </c>
     </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H13" t="s">
+        <v>15</v>
+      </c>
+      <c r="I13">
+        <f>(I9-I7)/2</f>
+        <v>6.700000000000006E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H14" t="s">
+        <v>16</v>
+      </c>
+      <c r="I14">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="D1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="2"/>
+      <c r="G1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" s="2"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3">
+        <v>0.47</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3">
+        <v>0.42</v>
+      </c>
+      <c r="G3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4">
+        <v>0.53700000000000003</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="G4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4">
+        <v>0.61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5">
+        <v>0.73</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5">
+        <v>0.73</v>
+      </c>
+      <c r="G5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5">
+        <v>0.78518518518518499</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6">
+        <f>20</f>
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6">
+        <f>20</f>
+        <v>20</v>
+      </c>
+      <c r="G6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6">
+        <f>20</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8">
+        <v>29</v>
+      </c>
+      <c r="D8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8">
+        <v>29</v>
+      </c>
+      <c r="G8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10">
+        <f>B5*2</f>
+        <v>1.46</v>
+      </c>
+      <c r="D10" t="s">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <f>E5*2</f>
+        <v>1.46</v>
+      </c>
+      <c r="G10" t="s">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <f>H5*2</f>
+        <v>1.57037037037037</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <f>B10*42.4</f>
+        <v>61.903999999999996</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <f>E10*42.4</f>
+        <v>61.903999999999996</v>
+      </c>
+      <c r="G11" t="s">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <f>H10*42.4</f>
+        <v>66.583703703703691</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <f>B3*2</f>
+        <v>0.94</v>
+      </c>
+      <c r="D12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12">
+        <f>E3*2</f>
+        <v>0.84</v>
+      </c>
+      <c r="G12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12">
+        <f>H3*2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13">
+        <f>B12*20.943*2</f>
+        <v>39.372840000000004</v>
+      </c>
+      <c r="D13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13">
+        <f>E12*20.943*2</f>
+        <v>35.184240000000003</v>
+      </c>
+      <c r="G13" t="s">
+        <v>3</v>
+      </c>
+      <c r="H13">
+        <f>H12*20.943*2</f>
+        <v>41.886000000000003</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <f>B4*2</f>
+        <v>1.0740000000000001</v>
+      </c>
+      <c r="D14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14">
+        <f>E4*2</f>
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="G14" t="s">
+        <v>12</v>
+      </c>
+      <c r="H14">
+        <f>H4*2</f>
+        <v>1.22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <f>B14*42.4</f>
+        <v>45.537600000000005</v>
+      </c>
+      <c r="D15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15">
+        <f>E14*42.4</f>
+        <v>48.335999999999991</v>
+      </c>
+      <c r="G15" t="s">
+        <v>13</v>
+      </c>
+      <c r="H15">
+        <f>H14*42.4</f>
+        <v>51.727999999999994</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16">
+        <f>B11-B15</f>
+        <v>16.366399999999992</v>
+      </c>
+      <c r="D16" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16">
+        <f>E11-E15</f>
+        <v>13.568000000000005</v>
+      </c>
+      <c r="G16" t="s">
+        <v>7</v>
+      </c>
+      <c r="H16">
+        <f>H11-H15</f>
+        <v>14.855703703703696</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="3">
+        <f>B13/B16</f>
+        <v>2.4057117020236598</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="3">
+        <f>E13/E16</f>
+        <v>2.5931780660377353</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H17" s="3">
+        <f>H13/H16</f>
+        <v>2.8195231161992917</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19">
+        <f>(B14-B12)/2</f>
+        <v>6.700000000000006E-2</v>
+      </c>
+      <c r="D19" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19">
+        <f>(E14-E12)/2</f>
+        <v>0.14999999999999997</v>
+      </c>
+      <c r="G19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H19">
+        <f>(H14-H12)/2</f>
+        <v>0.10999999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20">
+        <f>(B5-B4)*2</f>
+        <v>0.3859999999999999</v>
+      </c>
+      <c r="D20" t="s">
+        <v>29</v>
+      </c>
+      <c r="E20">
+        <f>(E5-E4)*2</f>
+        <v>0.32000000000000006</v>
+      </c>
+      <c r="G20" t="s">
+        <v>29</v>
+      </c>
+      <c r="H20">
+        <f>(H5-H4)*2</f>
+        <v>0.35037037037037</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21">
+        <f>B13*B6*B8</f>
+        <v>22836.247200000002</v>
+      </c>
+      <c r="D21" t="s">
+        <v>25</v>
+      </c>
+      <c r="E21">
+        <f>E13*E6*E8</f>
+        <v>20406.859199999999</v>
+      </c>
+      <c r="G21" t="s">
+        <v>25</v>
+      </c>
+      <c r="H21">
+        <f>H13*H6*H8</f>
+        <v>22618.440000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22">
+        <f>273</f>
+        <v>273</v>
+      </c>
+      <c r="D22" t="s">
+        <v>27</v>
+      </c>
+      <c r="E22">
+        <v>273</v>
+      </c>
+      <c r="G22" t="s">
+        <v>27</v>
+      </c>
+      <c r="H22">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23">
+        <f>B21*B22</f>
+        <v>6234295.4856000002</v>
+      </c>
+      <c r="D23" t="s">
+        <v>28</v>
+      </c>
+      <c r="E23">
+        <f>E21*E22</f>
+        <v>5571072.5615999997</v>
+      </c>
+      <c r="G23" t="s">
+        <v>28</v>
+      </c>
+      <c r="H23">
+        <f>H21*H22</f>
+        <v>6174834.120000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="G1:H1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>